<commit_message>
Actualización Matriz control de cambios
</commit_message>
<xml_diff>
--- a/Documentos/2 Control de Cambios/MATRIZ CONTROL DE CAMBIO.xlsx
+++ b/Documentos/2 Control de Cambios/MATRIZ CONTROL DE CAMBIO.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProyectoCIDEF\Documentos\2 Control de Cambios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAF5B6D6-1F9A-4808-8090-C26854AF225F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="270" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -34,15 +40,6 @@
   </si>
   <si>
     <t>SC-01</t>
-  </si>
-  <si>
-    <t>SC-02</t>
-  </si>
-  <si>
-    <t>SC-03</t>
-  </si>
-  <si>
-    <t>SC-04</t>
   </si>
   <si>
     <t>Fase del Proyecto en que se Aplica</t>
@@ -72,9 +69,6 @@
 Aceptado-Rechazado</t>
   </si>
   <si>
-    <t>Que la pagina muestre fotos de la compañía</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -84,94 +78,34 @@
     <t>Medio</t>
   </si>
   <si>
-    <t>Diseño</t>
-  </si>
-  <si>
     <t>Aceptado</t>
   </si>
   <si>
     <t>SC</t>
   </si>
   <si>
-    <t>Alto</t>
-  </si>
-  <si>
-    <t>Agregar fotos a la pagina con respecto a la agencia.</t>
-  </si>
-  <si>
-    <t>Urgente</t>
-  </si>
-  <si>
     <t>Planificacion</t>
   </si>
   <si>
-    <t>Que se comprenda la informacion que se esta visualizando en la pagina</t>
-  </si>
-  <si>
-    <t>Requerimiento relacionado (RF-N°)</t>
-  </si>
-  <si>
-    <t>Caso de uso relacionado (CU-N°)</t>
-  </si>
-  <si>
-    <t>Permitir ver terminos y condiciones del viaje, incluyendo seguros</t>
-  </si>
-  <si>
-    <t>R.12</t>
-  </si>
-  <si>
-    <t>Mostrar un registro de los terminos y condiciones para los viajes, ademas deberá contener los seguros para los alumnos</t>
-  </si>
-  <si>
-    <t>Mayor claridad a la hora de mostrar la informacion</t>
-  </si>
-  <si>
-    <t>CU.005</t>
-  </si>
-  <si>
-    <t>CU.006</t>
-  </si>
-  <si>
-    <t>Validar si los datos se ingresaron correctamente al sistema</t>
-  </si>
-  <si>
-    <t>Dentro de la base de datos, consultar si estan los usuarios con sus pedidos</t>
-  </si>
-  <si>
-    <t>CU.001</t>
-  </si>
-  <si>
-    <t>R.8</t>
-  </si>
-  <si>
-    <t>R.9</t>
-  </si>
-  <si>
-    <t>R.6</t>
-  </si>
-  <si>
-    <t>SC-05</t>
-  </si>
-  <si>
-    <t>R.13</t>
-  </si>
-  <si>
-    <t>CU.008</t>
-  </si>
-  <si>
-    <t>El dueño debe poder consultar el avance de los colegios en actividades</t>
-  </si>
-  <si>
-    <t>Dentro del sistema, el dueño de la agencia podrá consultar el porcentaje de avance logrado, de actividades realizadas por colegios y sus cursos</t>
-  </si>
-  <si>
-    <t>CU.009</t>
+    <t>Apartados para nivel básico y experto</t>
+  </si>
+  <si>
+    <t>Agregar un inicio con selección según tipo de usuario, el se divide en básico (personas con bajo conocimiento en repuestos) y experto (personas con conocimientos en repuestos de vehiculos)</t>
+  </si>
+  <si>
+    <t>Sacar del formulario el RUT y dejar seleccionable el asunto</t>
+  </si>
+  <si>
+    <t>En el formulario de contacto, no permitir que se escriba en el asunto del correo, además, quitar el campo que solicita RUT del cliente.</t>
+  </si>
+  <si>
+    <t>C-02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,12 +351,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -441,21 +371,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -468,6 +383,30 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -781,18 +720,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,31 +743,27 @@
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
+    <row r="1" spans="2:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
     </row>
-    <row r="2" spans="2:13" s="1" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:11" s="21" customFormat="1" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -837,241 +772,143 @@
       <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="13" t="s">
+    </row>
+    <row r="3" spans="2:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44225</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="7">
+        <v>44225</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="F4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="H4" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="2:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="5">
-        <v>44015</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>20</v>
-      </c>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="6"/>
     </row>
-    <row r="4" spans="2:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="9">
-        <v>44023</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="8" t="s">
-        <v>20</v>
-      </c>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="6"/>
     </row>
-    <row r="5" spans="2:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="9">
-        <v>44052</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>20</v>
-      </c>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="6"/>
     </row>
-    <row r="6" spans="2:13" ht="135" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="9">
-        <v>44083</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="9">
-        <v>44157</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="17"/>
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:M1"/>
+    <mergeCell ref="B1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>

</xml_diff>